<commit_message>
Added ACHCorporate Reusable Library, Added TestCase for PayNowCorporate
</commit_message>
<xml_diff>
--- a/KatalonData/IWPTestData/VRelay25Payments.xlsx
+++ b/KatalonData/IWPTestData/VRelay25Payments.xlsx
@@ -1,23 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\IWPTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{01F2B10C-9D77-4A1A-8D5C-2F81C8C46C50}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F7D13A-9DAC-4F0C-AC91-DF3601B3EA9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView windowHeight="16920" windowWidth="30960" xWindow="30600" xr2:uid="{E8C53DAE-1554-4E2D-AB4B-2AFBF084D73A}" yWindow="-120"/>
+    <workbookView xWindow="795" yWindow="975" windowWidth="18105" windowHeight="10800" activeTab="2" xr2:uid="{E8C53DAE-1554-4E2D-AB4B-2AFBF084D73A}"/>
   </bookViews>
   <sheets>
-    <sheet name="PayNowCC" r:id="rId1" sheetId="1"/>
+    <sheet name="PayNowCC" sheetId="1" r:id="rId1"/>
+    <sheet name="PayNowPC" sheetId="3" r:id="rId2"/>
+    <sheet name="PayNowPS" sheetId="4" r:id="rId3"/>
+    <sheet name="PayNowCorp" sheetId="2" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="96">
   <si>
     <t>Result</t>
   </si>
@@ -122,9 +125,6 @@
     <t>CCEmail</t>
   </si>
   <si>
-    <t>Pay Now Credit Card</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -140,29 +140,199 @@
     <t>2028</t>
   </si>
   <si>
-    <t>831</t>
-  </si>
-  <si>
     <t>2.5</t>
   </si>
   <si>
     <t>8</t>
   </si>
   <si>
-    <t/>
-  </si>
-  <si>
     <t>Pass</t>
   </si>
   <si>
     <t>Thu Aug 08 14:18:38 EDT 2024</t>
+  </si>
+  <si>
+    <t>ACNumber</t>
+  </si>
+  <si>
+    <t>CompanyName</t>
+  </si>
+  <si>
+    <t>EIN</t>
+  </si>
+  <si>
+    <t>Amount</t>
+  </si>
+  <si>
+    <t>UDF1</t>
+  </si>
+  <si>
+    <t>UDF2</t>
+  </si>
+  <si>
+    <t>UDF3</t>
+  </si>
+  <si>
+    <t>UDF4</t>
+  </si>
+  <si>
+    <t>UDF5</t>
+  </si>
+  <si>
+    <t>UDF6</t>
+  </si>
+  <si>
+    <t>UDF7</t>
+  </si>
+  <si>
+    <t>UDF8</t>
+  </si>
+  <si>
+    <t>UDF9</t>
+  </si>
+  <si>
+    <t>UDF10</t>
+  </si>
+  <si>
+    <t>AL1</t>
+  </si>
+  <si>
+    <t>AL2</t>
+  </si>
+  <si>
+    <t>ZIP</t>
+  </si>
+  <si>
+    <t>Email</t>
+  </si>
+  <si>
+    <t>RTN</t>
+  </si>
+  <si>
+    <t>My Company</t>
+  </si>
+  <si>
+    <t>10</t>
+  </si>
+  <si>
+    <t>Pay Now Corporate No Emulator Data</t>
+  </si>
+  <si>
+    <t>Pay Now Corporate Yes Emulator Data</t>
+  </si>
+  <si>
+    <t>638</t>
+  </si>
+  <si>
+    <t>Pay Now Credit Card Yes Emulator Data</t>
+  </si>
+  <si>
+    <t>Pay Now Credit Card No Emulator Data</t>
+  </si>
+  <si>
+    <t>10.50</t>
+  </si>
+  <si>
+    <t>udf data 1</t>
+  </si>
+  <si>
+    <t>udf data 2</t>
+  </si>
+  <si>
+    <t>udf data 3</t>
+  </si>
+  <si>
+    <t>udf data 4</t>
+  </si>
+  <si>
+    <t>udf data 5</t>
+  </si>
+  <si>
+    <t>udf data 6</t>
+  </si>
+  <si>
+    <t>Orange</t>
+  </si>
+  <si>
+    <t>Soccer</t>
+  </si>
+  <si>
+    <t>udf data 9</t>
+  </si>
+  <si>
+    <t>udf data 10</t>
+  </si>
+  <si>
+    <t>Kavita Ranawati</t>
+  </si>
+  <si>
+    <t>4111111111111111</t>
+  </si>
+  <si>
+    <t>365 Main Avenue</t>
+  </si>
+  <si>
+    <t>22201</t>
+  </si>
+  <si>
+    <t>iahmed@govolution.com</t>
+  </si>
+  <si>
+    <t>Charu Suraji</t>
+  </si>
+  <si>
+    <t>374245002771003</t>
+  </si>
+  <si>
+    <t>1234</t>
+  </si>
+  <si>
+    <t>Pay Now Corporate No Emulator Data Required Fields Only</t>
+  </si>
+  <si>
+    <t>Pay Now Credit Card No Emulator Data Required Fields only</t>
+  </si>
+  <si>
+    <t>Shakuntla Devi</t>
+  </si>
+  <si>
+    <t>Fname</t>
+  </si>
+  <si>
+    <t>Lname</t>
+  </si>
+  <si>
+    <t>ConfirmACNumber</t>
+  </si>
+  <si>
+    <t>ACType</t>
+  </si>
+  <si>
+    <t>Pay Now PC No Emulator Data</t>
+  </si>
+  <si>
+    <t>Pay Now PC Yes Emulator Data</t>
+  </si>
+  <si>
+    <t>Pay Now PC No Emulator Data Required Fields Only</t>
+  </si>
+  <si>
+    <t>12342222</t>
+  </si>
+  <si>
+    <t>CACNumber</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -205,20 +375,25 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
+  <cellXfs count="4">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -235,10 +410,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr lastClr="000000" val="windowText"/>
+        <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr lastClr="FFFFFF" val="window"/>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -273,7 +448,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin panose="02110004020202020204" typeface="Aptos Display"/>
+        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -325,7 +500,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin panose="02110004020202020204" typeface="Aptos Narrow"/>
+        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -436,21 +611,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
+        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
+        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -467,7 +642,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
+            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -539,44 +714,45 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" name="Office Theme" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6645B547-9B3F-42C0-A45B-8EF8C475631F}">
-  <dimension ref="A1:AC2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6645B547-9B3F-42C0-A45B-8EF8C475631F}">
+  <dimension ref="A1:AB5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+    <sheetView topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="AC1" sqref="AC1:AC1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" bestFit="true" customWidth="true" style="2" width="6.42578125" collapsed="false"/>
-    <col min="2" max="2" bestFit="true" customWidth="true" style="2" width="27.5703125" collapsed="false"/>
-    <col min="3" max="3" bestFit="true" customWidth="true" style="2" width="19.0" collapsed="false"/>
-    <col min="4" max="4" bestFit="true" customWidth="true" style="2" width="7.5703125" collapsed="false"/>
-    <col min="5" max="5" bestFit="true" customWidth="true" style="2" width="9.0" collapsed="false"/>
-    <col min="6" max="6" bestFit="true" customWidth="true" style="2" width="6.28515625" collapsed="false"/>
-    <col min="7" max="7" bestFit="true" customWidth="true" style="2" width="8.7109375" collapsed="false"/>
-    <col min="8" max="8" customWidth="true" style="2" width="13.42578125" collapsed="false"/>
-    <col min="9" max="17" bestFit="true" customWidth="true" style="2" width="7.85546875" collapsed="false"/>
-    <col min="18" max="18" bestFit="true" customWidth="true" style="2" width="8.85546875" collapsed="false"/>
-    <col min="19" max="19" bestFit="true" customWidth="true" style="2" width="8.5703125" collapsed="false"/>
-    <col min="20" max="20" bestFit="true" customWidth="true" style="2" width="17.28515625" collapsed="false"/>
-    <col min="21" max="21" bestFit="true" customWidth="true" style="2" width="6.5703125" collapsed="false"/>
-    <col min="22" max="22" bestFit="true" customWidth="true" style="2" width="7.85546875" collapsed="false"/>
-    <col min="23" max="24" bestFit="true" customWidth="true" style="2" width="7.28515625" collapsed="false"/>
-    <col min="25" max="26" bestFit="true" customWidth="true" style="2" width="6.28515625" collapsed="false"/>
-    <col min="27" max="27" bestFit="true" customWidth="true" style="2" width="6.0" collapsed="false"/>
-    <col min="28" max="28" bestFit="true" customWidth="true" style="2" width="8.28515625" collapsed="false"/>
-    <col min="29" max="16384" style="2" width="9.140625" collapsed="false"/>
+    <col min="1" max="1" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19" style="1" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="9" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.42578125" style="1" customWidth="1"/>
+    <col min="9" max="17" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="17.42578125" style="1" customWidth="1"/>
+    <col min="20" max="20" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="13" style="1" customWidth="1"/>
+    <col min="26" max="26" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="14.7109375" style="1" customWidth="1"/>
+    <col min="29" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1" ht="30" r="1" s="1" spans="1:28" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:28" ht="30" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -662,46 +838,1111 @@
         <v>27</v>
       </c>
     </row>
-    <row customFormat="1" r="2" s="1" spans="1:28" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>38</v>
-      </c>
-      <c r="B2" t="s">
-        <v>39</v>
+    <row r="2" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>36</v>
       </c>
       <c r="C2" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="T2" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="E2" s="1" t="s">
-        <v>36</v>
-      </c>
-      <c r="F2" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="T2" s="1" t="s">
+      <c r="U2" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="U2" s="1" t="s">
+      <c r="V2" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="V2" s="1" t="s">
+      <c r="W2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="W2" s="1" t="s">
+    </row>
+    <row r="3" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="AB2" s="2"/>
+      <c r="H3" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I3" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J3" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K3" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L3" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M3" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N3" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O3" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q3" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="R3" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="S3" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="T3" s="1" t="s">
+        <v>75</v>
+      </c>
+      <c r="U3" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y3" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA3" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB3" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I4" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J4" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N4" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O4" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="T4" s="1" t="s">
+        <v>80</v>
+      </c>
+      <c r="U4" s="1" t="s">
+        <v>81</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB4" s="3" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="5" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+      <c r="C5" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="D5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E5" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H5" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K5" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L5" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M5" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="P5" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q5" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="R5" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="S5" s="1" t="s">
+        <v>84</v>
+      </c>
+      <c r="T5" s="1" t="s">
+        <v>29</v>
+      </c>
+      <c r="U5" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>31</v>
+      </c>
+      <c r="W5" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="Y5" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA5" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB5" s="3" t="s">
+        <v>78</v>
+      </c>
     </row>
   </sheetData>
-  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6CB7062-F3FE-4F59-AAD7-F881C9AC66C0}">
+  <dimension ref="A1:AB4"/>
+  <sheetViews>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="X4" sqref="X4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="14" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="10.7109375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="10.42578125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="U2" s="1">
+        <v>256072691</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="U3" s="1">
+        <v>256072691</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="U4" s="1">
+        <v>256072691</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>94</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE1C1C0F-53C1-43E2-B9A2-9B1C832B80B6}">
+  <dimension ref="A1:AB4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="X4" sqref="X4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="14" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="10.7109375" style="1" customWidth="1"/>
+    <col min="21" max="21" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="23" max="24" width="10.42578125" style="1" customWidth="1"/>
+    <col min="25" max="25" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="29" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>85</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>86</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>88</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AB1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>89</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="U2" s="1">
+        <v>256072691</v>
+      </c>
+      <c r="V2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="W2" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB2" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="U3" s="1">
+        <v>256072691</v>
+      </c>
+      <c r="V3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="W3" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="X3" s="1" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>91</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="U4" s="1">
+        <v>256072691</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="W4" s="1" t="s">
+        <v>92</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>95</v>
+      </c>
+      <c r="Y4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AB4" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B1D5DBD-8D22-4B19-B9D2-FF1FC12487BE}">
+  <dimension ref="A1:AA4"/>
+  <sheetViews>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="P3" sqref="P3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="26.85546875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="14" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.140625" style="1" customWidth="1"/>
+    <col min="23" max="23" width="10" style="1" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="4" style="1" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="6" style="1" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="9.140625" style="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>40</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>41</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>42</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="P1" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>50</v>
+      </c>
+      <c r="S1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T1" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="U1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="V1" s="1" t="s">
+        <v>93</v>
+      </c>
+      <c r="W1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="X1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Y1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z1" s="1" t="s">
+        <v>53</v>
+      </c>
+      <c r="AA1" s="1" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+      <c r="C2" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="D2" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G2" s="1">
+        <v>2.5</v>
+      </c>
+      <c r="H2" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="I2" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="J2" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="K2" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L2" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M2" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="N2" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="O2" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="P2" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q2" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="R2" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="S2" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T2" s="1">
+        <v>256072691</v>
+      </c>
+      <c r="U2" s="1">
+        <v>12344444</v>
+      </c>
+      <c r="V2" s="1">
+        <v>12344444</v>
+      </c>
+      <c r="W2" s="1">
+        <v>123456789</v>
+      </c>
+      <c r="X2" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z2" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA2" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+      <c r="C3" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="P3" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="T3" s="1">
+        <v>256072691</v>
+      </c>
+      <c r="U3" s="1">
+        <v>12344444</v>
+      </c>
+      <c r="V3" s="1">
+        <v>12344444</v>
+      </c>
+      <c r="W3" s="1">
+        <v>123456789</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+      <c r="C4" s="1" t="s">
+        <v>82</v>
+      </c>
+      <c r="D4" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="E4" s="1" t="s">
+        <v>57</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="K4" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="L4" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="M4" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="P4" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="Q4" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="R4" s="1" t="s">
+        <v>73</v>
+      </c>
+      <c r="S4" s="1" t="s">
+        <v>56</v>
+      </c>
+      <c r="T4" s="1">
+        <v>256072691</v>
+      </c>
+      <c r="U4" s="1">
+        <v>12344444</v>
+      </c>
+      <c r="V4" s="1">
+        <v>12344444</v>
+      </c>
+      <c r="X4" s="1" t="s">
+        <v>76</v>
+      </c>
+      <c r="Z4" s="1" t="s">
+        <v>77</v>
+      </c>
+      <c r="AA4" s="1" t="s">
+        <v>78</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Modified Emulator data file
</commit_message>
<xml_diff>
--- a/KatalonData/IWPTestData/VRelay25Payments.xlsx
+++ b/KatalonData/IWPTestData/VRelay25Payments.xlsx
@@ -1,26 +1,26 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27628"/>
   <workbookPr defaultThemeVersion="202300"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Cloned-Project-Katalon\VPS-Katalon\KatalonData\IWPTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65F7D13A-9DAC-4F0C-AC91-DF3601B3EA9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr documentId="13_ncr:1_{65F7D13A-9DAC-4F0C-AC91-DF3601B3EA9C}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView xWindow="795" yWindow="975" windowWidth="18105" windowHeight="10800" activeTab="2" xr2:uid="{E8C53DAE-1554-4E2D-AB4B-2AFBF084D73A}"/>
+    <workbookView activeTab="2" windowHeight="10800" windowWidth="18105" xWindow="795" xr2:uid="{E8C53DAE-1554-4E2D-AB4B-2AFBF084D73A}" yWindow="975"/>
   </bookViews>
   <sheets>
-    <sheet name="PayNowCC" sheetId="1" r:id="rId1"/>
-    <sheet name="PayNowPC" sheetId="3" r:id="rId2"/>
-    <sheet name="PayNowPS" sheetId="4" r:id="rId3"/>
-    <sheet name="PayNowCorp" sheetId="2" r:id="rId4"/>
+    <sheet name="PayNowCC" r:id="rId1" sheetId="1"/>
+    <sheet name="PayNowPC" r:id="rId2" sheetId="3"/>
+    <sheet name="PayNowPS" r:id="rId3" sheetId="4"/>
+    <sheet name="PayNowCorp" r:id="rId4" sheetId="2"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
+    <ext uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="325" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="100">
   <si>
     <t>Result</t>
   </si>
@@ -327,12 +327,25 @@
   </si>
   <si>
     <t>2</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>Thu Aug 15 22:14:55 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Aug 15 22:16:21 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Aug 15 22:17:32 IST 2024</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="0"/>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -375,25 +388,25 @@
     </border>
   </borders>
   <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
   <cellXfs count="4">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
+    <xf applyAlignment="1" applyBorder="1" applyNumberFormat="1" borderId="1" fillId="0" fontId="0" numFmtId="49" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf applyAlignment="1" borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf applyAlignment="1" applyBorder="1" borderId="1" fillId="0" fontId="0" numFmtId="0" xfId="0">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle builtinId="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium2"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -410,10 +423,10 @@
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
-        <a:sysClr val="windowText" lastClr="000000"/>
+        <a:sysClr lastClr="000000" val="windowText"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr lastClr="FFFFFF" val="window"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="0E2841"/>
@@ -448,7 +461,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Aptos Display" panose="02110004020202020204"/>
+        <a:latin panose="02110004020202020204" typeface="Aptos Display"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -500,7 +513,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Aptos Narrow" panose="02110004020202020204"/>
+        <a:latin panose="02110004020202020204" typeface="Aptos Narrow"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -611,21 +624,21 @@
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
-        <a:ln w="12700" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="12700">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="19050" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="19050">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
           <a:prstDash val="solid"/>
           <a:miter lim="800000"/>
         </a:ln>
-        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+        <a:ln algn="ctr" cap="flat" cmpd="sng" w="25400">
           <a:solidFill>
             <a:schemeClr val="phClr"/>
           </a:solidFill>
@@ -642,7 +655,7 @@
         </a:effectStyle>
         <a:effectStyle>
           <a:effectLst>
-            <a:outerShdw blurRad="57150" dist="19050" dir="5400000" algn="ctr" rotWithShape="0">
+            <a:outerShdw algn="ctr" blurRad="57150" dir="5400000" dist="19050" rotWithShape="0">
               <a:srgbClr val="000000">
                 <a:alpha val="63000"/>
               </a:srgbClr>
@@ -714,15 +727,15 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" id="{2E142A2C-CD16-42D6-873A-C26D2A0506FA}" name="Office Theme" vid="{1BDDFF52-6CD6-40A5-AB3C-68EB2F1E4D0A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6645B547-9B3F-42C0-A45B-8EF8C475631F}">
-  <dimension ref="A1:AB5"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6645B547-9B3F-42C0-A45B-8EF8C475631F}">
+  <dimension ref="A1:AC5"/>
   <sheetViews>
     <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="AC1" sqref="AC1:AC1048576"/>
@@ -730,29 +743,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19" style="1" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.42578125" style="1" customWidth="1"/>
-    <col min="9" max="17" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="8.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="17.42578125" style="1" customWidth="1"/>
-    <col min="20" max="20" width="17.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="7.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="13" style="1" customWidth="1"/>
-    <col min="26" max="26" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="14.7109375" style="1" customWidth="1"/>
-    <col min="29" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="27.5703125" collapsed="true"/>
+    <col min="3" max="3" bestFit="true" customWidth="true" style="1" width="19.0" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="7.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="9.0" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="8.7109375" collapsed="true"/>
+    <col min="8" max="8" customWidth="true" style="1" width="13.42578125" collapsed="true"/>
+    <col min="9" max="17" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="8.85546875" collapsed="true"/>
+    <col min="19" max="19" customWidth="true" style="1" width="17.42578125" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="17.28515625" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="6.5703125" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="23" max="24" bestFit="true" customWidth="true" style="1" width="7.28515625" collapsed="true"/>
+    <col min="25" max="25" customWidth="true" style="1" width="13.0" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
+    <col min="28" max="28" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="29" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -838,7 +851,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>35</v>
       </c>
@@ -873,7 +886,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>62</v>
       </c>
@@ -947,7 +960,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>62</v>
       </c>
@@ -1021,7 +1034,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="5" spans="1:28" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="5" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C5" s="1" t="s">
         <v>83</v>
       </c>
@@ -1084,7 +1097,7 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
   <headerFooter>
     <oddFooter xml:space="preserve">&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;K000000 Public </oddFooter>
   </headerFooter>
@@ -1092,8 +1105,8 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6CB7062-F3FE-4F59-AAD7-F881C9AC66C0}">
-  <dimension ref="A1:AB4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6CB7062-F3FE-4F59-AAD7-F881C9AC66C0}">
+  <dimension ref="A1:AC4"/>
   <sheetViews>
     <sheetView topLeftCell="N1" workbookViewId="0">
       <selection activeCell="X4" sqref="X4"/>
@@ -1101,31 +1114,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="14" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="10.7109375" style="1" customWidth="1"/>
-    <col min="21" max="21" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="10.42578125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="26.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="7.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="13.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="9" max="14" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="10.7109375" collapsed="true"/>
+    <col min="19" max="20" customWidth="true" style="1" width="10.7109375" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="23" max="24" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="15.7109375" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="4.0" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="23.5703125" collapsed="true"/>
+    <col min="29" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1211,7 +1224,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>89</v>
       </c>
@@ -1282,7 +1295,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>90</v>
       </c>
@@ -1311,7 +1324,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>91</v>
       </c>
@@ -1371,13 +1384,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE1C1C0F-53C1-43E2-B9A2-9B1C832B80B6}">
-  <dimension ref="A1:AB4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE1C1C0F-53C1-43E2-B9A2-9B1C832B80B6}">
+  <dimension ref="A1:AC4"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="M1" workbookViewId="0">
       <selection activeCell="X4" sqref="X4"/>
@@ -1385,31 +1398,31 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="14" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="10.7109375" style="1" customWidth="1"/>
-    <col min="21" max="21" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="23" max="24" width="10.42578125" style="1" customWidth="1"/>
-    <col min="25" max="25" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="29" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="26.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="7.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="13.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="9" max="14" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="10.7109375" collapsed="true"/>
+    <col min="19" max="20" customWidth="true" style="1" width="10.7109375" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="22" max="22" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="23" max="24" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="15.7109375" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="4.0" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
+    <col min="28" max="28" bestFit="true" customWidth="true" style="1" width="23.5703125" collapsed="true"/>
+    <col min="29" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="1" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1495,7 +1508,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="2" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C2" s="1" t="s">
         <v>89</v>
       </c>
@@ -1566,7 +1579,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="3" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C3" s="1" t="s">
         <v>90</v>
       </c>
@@ -1595,7 +1608,7 @@
         <v>95</v>
       </c>
     </row>
-    <row r="4" spans="1:28" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="4" spans="1:28" x14ac:dyDescent="0.25">
       <c r="C4" s="1" t="s">
         <v>91</v>
       </c>
@@ -1655,13 +1668,13 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B1D5DBD-8D22-4B19-B9D2-FF1FC12487BE}">
-  <dimension ref="A1:AA4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0B1D5DBD-8D22-4B19-B9D2-FF1FC12487BE}">
+  <dimension ref="A1:AB4"/>
   <sheetViews>
     <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="P3" sqref="P3"/>
@@ -1669,29 +1682,29 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="5" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="26.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="7.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="6.28515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="15.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="7.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="14" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="7.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.85546875" style="1" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="10.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.42578125" style="1" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.140625" style="1" customWidth="1"/>
-    <col min="23" max="23" width="10" style="1" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.7109375" style="1" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="4" style="1" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="6" style="1" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="23.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="28" max="16384" width="9.140625" style="1"/>
+    <col min="1" max="1" bestFit="true" customWidth="true" style="1" width="6.42578125" collapsed="true"/>
+    <col min="2" max="2" bestFit="true" customWidth="true" style="1" width="5.0" collapsed="true"/>
+    <col min="3" max="3" customWidth="true" style="1" width="26.85546875" collapsed="true"/>
+    <col min="4" max="4" bestFit="true" customWidth="true" style="1" width="7.5703125" collapsed="true"/>
+    <col min="5" max="5" bestFit="true" customWidth="true" style="1" width="13.28515625" collapsed="true"/>
+    <col min="6" max="6" bestFit="true" customWidth="true" style="1" width="6.28515625" collapsed="true"/>
+    <col min="7" max="7" bestFit="true" customWidth="true" style="1" width="15.5703125" collapsed="true"/>
+    <col min="8" max="8" bestFit="true" customWidth="true" style="1" width="7.85546875" collapsed="true"/>
+    <col min="9" max="14" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="15" max="15" bestFit="true" customWidth="true" style="1" width="7.42578125" collapsed="true"/>
+    <col min="16" max="16" bestFit="true" customWidth="true" style="1" width="6.85546875" collapsed="true"/>
+    <col min="17" max="17" bestFit="true" customWidth="true" style="1" width="9.7109375" collapsed="true"/>
+    <col min="18" max="18" bestFit="true" customWidth="true" style="1" width="10.7109375" collapsed="true"/>
+    <col min="19" max="19" bestFit="true" customWidth="true" style="1" width="14.7109375" collapsed="true"/>
+    <col min="20" max="20" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="21" max="21" bestFit="true" customWidth="true" style="1" width="10.42578125" collapsed="true"/>
+    <col min="22" max="22" customWidth="true" style="1" width="15.140625" collapsed="true"/>
+    <col min="23" max="23" bestFit="true" customWidth="true" style="1" width="10.0" collapsed="true"/>
+    <col min="24" max="24" bestFit="true" customWidth="true" style="1" width="15.7109375" collapsed="true"/>
+    <col min="25" max="25" bestFit="true" customWidth="true" style="1" width="4.0" collapsed="true"/>
+    <col min="26" max="26" bestFit="true" customWidth="true" style="1" width="6.0" collapsed="true"/>
+    <col min="27" max="27" bestFit="true" customWidth="true" style="1" width="23.5703125" collapsed="true"/>
+    <col min="28" max="16384" style="1" width="9.140625" collapsed="true"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:27" x14ac:dyDescent="0.25">
@@ -1777,7 +1790,13 @@
         <v>54</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="2" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" t="s">
+        <v>97</v>
+      </c>
       <c r="C2" s="1" t="s">
         <v>58</v>
       </c>
@@ -1851,7 +1870,13 @@
         <v>78</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="30" x14ac:dyDescent="0.25">
+    <row ht="30" r="3" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>35</v>
+      </c>
+      <c r="B3" t="s">
+        <v>98</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>59</v>
       </c>
@@ -1883,7 +1908,13 @@
         <v>123456789</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="45" x14ac:dyDescent="0.25">
+    <row ht="45" r="4" spans="1:27" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B4" t="s">
+        <v>99</v>
+      </c>
       <c r="C4" s="1" t="s">
         <v>82</v>
       </c>
@@ -1943,6 +1974,6 @@
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Deferred Test Cases and accessing excel sheet directly code
</commit_message>
<xml_diff>
--- a/KatalonData/IWPTestData/VRelay25Payments.xlsx
+++ b/KatalonData/IWPTestData/VRelay25Payments.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27830"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent>
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\t476046\Documents\katalon\VPS-Katalon\KatalonData\IWPTestData\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr documentId="13_ncr:1_{8FE73D97-94D6-41E0-9BFD-5E6E20F129FC}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
+  <xr:revisionPtr documentId="13_ncr:1_{D920EF28-2E9D-422F-9A2B-5D239D5EC53D}" revIDLastSave="0" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47"/>
   <bookViews>
-    <workbookView activeTab="7" firstSheet="3" tabRatio="980" windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
+    <workbookView activeTab="21" firstSheet="19" tabRatio="980" windowHeight="12576" windowWidth="23256" xWindow="-108" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}" yWindow="-108"/>
   </bookViews>
   <sheets>
     <sheet name="PayNowCC" r:id="rId1" sheetId="1"/>
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4384" uniqueCount="401">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3680" uniqueCount="238">
   <si>
     <t>Result</t>
   </si>
@@ -376,63 +376,6 @@
     <t>CCDate</t>
   </si>
   <si>
-    <t>Wed Sep 25 17:54:42 IST 2024</t>
-  </si>
-  <si>
-    <t>Wed Sep 25 17:56:05 IST 2024</t>
-  </si>
-  <si>
-    <t>Wed Sep 25 17:57:17 IST 2024</t>
-  </si>
-  <si>
-    <t>Wed Sep 25 17:58:29 IST 2024</t>
-  </si>
-  <si>
-    <t>Wed Sep 25 17:59:43 IST 2024</t>
-  </si>
-  <si>
-    <t>Wed Sep 25 18:00:57 IST 2024</t>
-  </si>
-  <si>
-    <t>Wed Sep 25 18:02:11 IST 2024</t>
-  </si>
-  <si>
-    <t>Wed Sep 25 18:03:22 IST 2024</t>
-  </si>
-  <si>
-    <t>Wed Sep 25 18:04:33 IST 2024</t>
-  </si>
-  <si>
-    <t>Wed Sep 25 18:05:46 IST 2024</t>
-  </si>
-  <si>
-    <t>Wed Sep 25 18:07:03 IST 2024</t>
-  </si>
-  <si>
-    <t>Wed Sep 25 18:08:00 IST 2024</t>
-  </si>
-  <si>
-    <t>Wed Sep 25 18:09:09 IST 2024</t>
-  </si>
-  <si>
-    <t>Wed Sep 25 18:10:16 IST 2024</t>
-  </si>
-  <si>
-    <t>Wed Sep 25 18:11:30 IST 2024</t>
-  </si>
-  <si>
-    <t>Wed Sep 25 18:12:39 IST 2024</t>
-  </si>
-  <si>
-    <t>Wed Sep 25 18:13:46 IST 2024</t>
-  </si>
-  <si>
-    <t>Wed Sep 25 18:14:56 IST 2024</t>
-  </si>
-  <si>
-    <t>Wed Sep 25 18:16:32 IST 2024</t>
-  </si>
-  <si>
     <t>4761730000000011</t>
   </si>
   <si>
@@ -463,817 +406,385 @@
     <t>825</t>
   </si>
   <si>
-    <t>Sat Oct 12 01:45:01 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 01:46:37 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 01:47:42 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 01:49:19 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 01:50:29 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 01:52:07 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 01:53:15 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 01:54:55 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 01:56:04 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 01:57:15 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 01:58:54 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:00:33 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:01:40 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:02:48 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:03:54 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:04:59 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:06:09 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:07:17 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:08:58 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:10:38 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:11:47 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:12:57 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:14:36 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:16:15 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:17:46 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:19:10 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:21:12 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:23:08 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:24:20 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:25:26 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:26:36 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:28:19 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:29:57 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:31:39 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:33:09 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:34:32 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:36:34 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:38:34 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:40:00 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:41:32 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:43:00 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:44:34 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:46:06 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:47:48 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:49:17 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:50:45 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:51:59 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:53:05 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:54:16 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:56:00 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 02:57:37 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 03:06:18 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 03:07:49 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 03:09:16 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 03:11:17 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 03:13:15 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 03:14:45 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 03:16:11 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 03:18:12 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 03:20:09 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 03:21:38 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 03:23:04 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 03:25:06 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 03:27:09 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 03:28:20 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 03:29:24 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 03:30:33 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 03:32:15 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 03:33:52 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 03:35:33 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 03:36:39 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 03:37:48 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 03:38:59 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 03:40:07 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 03:41:11 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 03:42:20 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 03:43:28 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 04:07:17 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 04:08:22 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 05:11:23 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 05:14:14 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 05:15:32 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 05:17:21 IST 2024</t>
-  </si>
-  <si>
-    <t>Sat Oct 12 05:20:34 IST 2024</t>
-  </si>
-  <si>
-    <t>Mon Oct 14 19:50:22 IST 2024</t>
-  </si>
-  <si>
     <t>Mon Oct 14 20:05:49 IST 2024</t>
   </si>
   <si>
+    <t>Tue Oct 15 06:50:33 IST 2024</t>
+  </si>
+  <si>
+    <t>Tue Oct 15 06:51:47 IST 2024</t>
+  </si>
+  <si>
+    <t>Tue Oct 15 06:52:52 IST 2024</t>
+  </si>
+  <si>
+    <t>Tue Oct 15 06:54:05 IST 2024</t>
+  </si>
+  <si>
+    <t>Tue Oct 15 06:55:53 IST 2024</t>
+  </si>
+  <si>
+    <t>Tue Oct 15 06:57:37 IST 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 23 19:09:25 IST 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 23 19:11:11 IST 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 23 19:13:28 IST 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 23 19:15:38 IST 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 23 19:24:44 IST 2024</t>
+  </si>
+  <si>
+    <t>Wed Oct 23 19:42:35 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 21:54:27 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 21:56:12 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 21:58:22 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:00:01 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:02:11 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:03:51 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:06:02 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:07:43 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:09:55 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:11:36 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:13:18 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:15:29 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:17:39 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:19:22 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:21:02 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:22:43 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:24:23 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:26:05 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:27:48 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:29:59 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:32:11 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:33:57 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:35:39 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:37:53 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:40:09 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:42:15 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:44:13 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:46:47 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:49:16 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:51:01 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:52:41 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:54:25 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:56:40 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 22:58:54 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:01:07 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:03:14 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:05:11 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:07:44 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:10:13 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:12:12 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:14:14 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:16:10 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:18:12 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:20:10 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:22:14 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:24:12 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:35:25 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:37:29 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:39:30 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:42:03 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:44:33 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:46:38 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:48:38 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:51:11 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:53:43 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:55:48 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Oct 24 23:57:47 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:00:21 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:02:51 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:04:31 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:06:16 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:08:03 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:09:47 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:11:25 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:13:08 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:14:54 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:33:24 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:34:58 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 00:36:38 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 01:18:22 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 01:20:10 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 01:21:56 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 01:23:43 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 01:26:00 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 01:27:57 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 01:30:24 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 01:32:24 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 02:36:05 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 02:37:54 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 02:39:38 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 02:41:22 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 02:46:33 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 02:48:18 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 02:50:04 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 02:51:59 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 02:53:43 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 02:55:27 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 02:57:08 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 02:58:52 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 03:00:34 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 03:02:18 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 03:03:59 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 03:05:44 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 03:07:24 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 03:09:09 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 03:10:49 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 03:12:20 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 03:13:49 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 03:15:29 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 03:17:07 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 03:18:47 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 03:20:24 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 03:22:04 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 03:23:42 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 03:25:21 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 03:26:59 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 03:28:39 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 03:30:18 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Oct 25 03:31:57 IST 2024</t>
+  </si>
+  <si>
+    <t>Mon Oct 28 19:52:54 IST 2024</t>
+  </si>
+  <si>
+    <t>Mon Oct 28 19:54:48 IST 2024</t>
+  </si>
+  <si>
+    <t>2000.50</t>
+  </si>
+  <si>
     <t/>
   </si>
   <si>
-    <t>Mon Oct 14 20:22:24 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 01:27:55 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 01:29:00 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 01:30:36 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 01:31:43 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 01:33:21 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 01:34:27 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 01:36:12 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 01:37:20 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 01:38:59 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 01:40:07 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 01:41:15 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 01:42:56 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 01:44:36 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 01:45:43 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 01:46:49 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 01:47:56 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 01:49:04 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 01:50:13 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 01:51:21 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 01:53:00 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 01:54:40 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 01:55:48 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 01:56:58 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 01:58:37 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:00:18 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:01:48 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:03:13 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:05:13 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:07:09 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:08:21 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:09:26 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:10:35 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:12:19 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:13:56 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:15:38 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:17:08 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:18:33 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:20:35 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:22:32 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:24:01 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:25:32 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:26:57 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:28:26 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:29:49 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:31:18 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:32:43 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:34:14 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:35:45 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:37:11 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:39:15 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:41:13 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:42:47 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:44:22 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:46:41 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:48:53 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:50:32 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:52:02 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:54:04 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:56:07 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:57:39 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 02:59:05 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 03:01:06 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 03:03:06 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 03:04:15 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 03:05:28 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 03:06:40 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 03:07:48 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 03:08:46 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 03:09:55 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 03:11:07 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 03:25:45 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 03:26:48 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 03:27:55 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 04:02:04 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 04:03:22 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 04:04:38 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 04:05:54 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 04:07:40 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 04:09:06 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 04:11:02 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 04:12:28 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:06:26 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:07:32 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:09:09 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:10:15 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:11:54 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:13:03 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:14:44 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:15:53 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:17:34 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:18:46 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:19:58 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:21:39 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:23:19 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:24:29 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:25:34 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:26:41 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:27:48 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:28:58 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:30:07 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:31:51 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:33:32 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:34:42 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:35:53 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:37:33 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:39:14 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:40:48 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:42:13 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:44:13 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:46:12 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:47:24 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:48:33 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:49:45 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:51:30 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:53:09 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:54:51 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:56:24 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:57:48 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 05:59:49 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:01:48 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:03:15 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:04:45 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:06:10 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:07:39 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:09:12 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:10:43 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:12:08 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:13:37 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:14:53 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:16:02 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:17:13 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:18:58 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:20:36 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:22:20 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:23:53 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:25:25 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:27:28 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:29:29 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:31:01 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:32:27 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:34:30 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:36:29 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:38:01 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:39:27 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:41:30 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:43:29 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:45:01 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:46:29 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:48:34 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:50:33 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:51:47 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:52:52 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:54:05 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:55:53 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:57:37 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 06:59:20 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 07:00:28 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 07:01:42 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 07:02:55 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 07:04:09 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 07:05:16 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 07:06:27 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 07:07:38 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 07:37:43 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 07:38:46 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 07:39:54 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 08:34:53 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 08:36:12 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 08:37:28 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 08:38:45 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 08:40:32 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 08:41:59 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 08:43:57 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 08:45:34 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 19:48:46 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 19:50:11 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 19:51:29 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 19:52:44 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 19:53:59 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 19:55:07 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 19:56:19 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 19:57:34 IST 2024</t>
-  </si>
-  <si>
-    <t>Tue Oct 15 21:03:50 IST 2024</t>
+    <t>Mon Nov 04 22:07:50 IST 2024</t>
   </si>
 </sst>
 </file>
@@ -1810,7 +1321,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>392</v>
+        <v>182</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -1848,7 +1359,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>393</v>
+        <v>183</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>16</v>
@@ -1928,7 +1439,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>394</v>
+        <v>184</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>16</v>
@@ -2008,7 +1519,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>395</v>
+        <v>185</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>37</v>
@@ -2076,7 +1587,7 @@
         <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>396</v>
+        <v>186</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
@@ -2085,13 +1596,13 @@
         <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>26</v>
@@ -2114,7 +1625,7 @@
         <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>397</v>
+        <v>187</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>16</v>
@@ -2123,13 +1634,13 @@
         <v>8</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>18</v>
@@ -2194,7 +1705,7 @@
         <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>398</v>
+        <v>188</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>16</v>
@@ -2203,13 +1714,13 @@
         <v>8</v>
       </c>
       <c r="E8" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H8" s="1" t="s">
         <v>18</v>
@@ -2274,7 +1785,7 @@
         <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>400</v>
+        <v>189</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>37</v>
@@ -2283,13 +1794,13 @@
         <v>8</v>
       </c>
       <c r="E9" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F9" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H9" s="1" t="s">
         <v>18</v>
@@ -2447,7 +1958,7 @@
         <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>215</v>
+        <v>111</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>16</v>
@@ -2529,7 +2040,7 @@
         <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>381</v>
+        <v>190</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>16</v>
@@ -2538,13 +2049,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>18</v>
@@ -2712,7 +2223,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>384</v>
+        <v>193</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>16</v>
@@ -2794,7 +2305,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>385</v>
+        <v>194</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>16</v>
@@ -2803,13 +2314,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>18</v>
@@ -3065,13 +2576,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>18</v>
@@ -3244,7 +2755,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>388</v>
+        <v>197</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>59</v>
@@ -3328,7 +2839,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>389</v>
+        <v>198</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>59</v>
@@ -3337,13 +2848,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>18</v>
@@ -3513,7 +3024,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>333</v>
+        <v>158</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>66</v>
@@ -3594,7 +3105,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>334</v>
+        <v>159</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>68</v>
@@ -3647,7 +3158,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>335</v>
+        <v>160</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>66</v>
@@ -3656,13 +3167,13 @@
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>18</v>
@@ -3728,7 +3239,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>336</v>
+        <v>161</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>68</v>
@@ -3737,13 +3248,13 @@
         <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -3887,7 +3398,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>341</v>
+        <v>166</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -3941,7 +3452,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>342</v>
+        <v>167</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>16</v>
@@ -4023,7 +3534,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>343</v>
+        <v>168</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -4032,13 +3543,13 @@
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -4077,7 +3588,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>344</v>
+        <v>169</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>16</v>
@@ -4086,13 +3597,13 @@
         <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>18</v>
@@ -4266,7 +3777,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>355</v>
+        <v>170</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>82</v>
@@ -4353,7 +3864,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>356</v>
+        <v>171</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>83</v>
@@ -4414,7 +3925,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>357</v>
+        <v>172</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>82</v>
@@ -4423,13 +3934,13 @@
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>18</v>
@@ -4501,7 +4012,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>358</v>
+        <v>173</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>83</v>
@@ -4510,13 +4021,13 @@
         <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -4669,7 +4180,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>363</v>
+        <v>178</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>82</v>
@@ -4756,7 +4267,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>364</v>
+        <v>179</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>83</v>
@@ -4817,7 +4328,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>365</v>
+        <v>180</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>82</v>
@@ -4826,13 +4337,13 @@
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>18</v>
@@ -4904,7 +4415,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>366</v>
+        <v>181</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>83</v>
@@ -4913,13 +4424,13 @@
         <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>125</v>
+        <v>106</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -5066,7 +4577,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>337</v>
+        <v>162</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -5098,7 +4609,7 @@
       <c r="R2" s="1"/>
       <c r="S2" s="1"/>
       <c r="T2" s="1" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="U2" s="1" t="s">
         <v>13</v>
@@ -5120,7 +4631,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>338</v>
+        <v>163</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>16</v>
@@ -5202,7 +4713,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>339</v>
+        <v>164</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -5211,13 +4722,13 @@
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" s="1"/>
@@ -5234,7 +4745,7 @@
       <c r="R4" s="1"/>
       <c r="S4" s="1"/>
       <c r="T4" s="1" t="s">
-        <v>120</v>
+        <v>101</v>
       </c>
       <c r="U4" s="1" t="s">
         <v>13</v>
@@ -5256,7 +4767,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>340</v>
+        <v>165</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>16</v>
@@ -5265,13 +4776,13 @@
         <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>18</v>
@@ -5439,7 +4950,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>323</v>
+        <v>148</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>66</v>
@@ -5520,7 +5031,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>324</v>
+        <v>149</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>68</v>
@@ -5573,7 +5084,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>325</v>
+        <v>150</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>66</v>
@@ -5582,13 +5093,13 @@
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>18</v>
@@ -5654,7 +5165,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>326</v>
+        <v>151</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>68</v>
@@ -5663,13 +5174,13 @@
         <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -5717,13 +5228,13 @@
   <dimension ref="A1:AD7"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
     <col min="1" max="1" customWidth="true" style="1" width="6.44140625" collapsed="true"/>
-    <col min="2" max="2" customWidth="true" style="1" width="5.0" collapsed="true"/>
+    <col min="2" max="2" customWidth="true" style="1" width="21.21875" collapsed="true"/>
     <col min="3" max="3" customWidth="true" style="1" width="26.77734375" collapsed="true"/>
     <col min="4" max="4" customWidth="true" style="1" width="7.5546875" collapsed="true"/>
     <col min="5" max="5" customWidth="true" style="1" width="13.21875" collapsed="true"/>
@@ -5838,7 +5349,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>345</v>
+        <v>122</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>59</v>
@@ -5921,7 +5432,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>346</v>
+        <v>123</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>61</v>
@@ -5959,7 +5470,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>347</v>
+        <v>118</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>62</v>
@@ -6030,7 +5541,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>348</v>
+        <v>119</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>59</v>
@@ -6039,13 +5550,13 @@
         <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>18</v>
@@ -6113,7 +5624,7 @@
         <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>349</v>
+        <v>120</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>61</v>
@@ -6122,13 +5633,13 @@
         <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>26</v>
@@ -6151,7 +5662,7 @@
         <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>350</v>
+        <v>121</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>62</v>
@@ -6160,13 +5671,13 @@
         <v>8</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>18</v>
@@ -6330,7 +5841,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>359</v>
+        <v>174</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>82</v>
@@ -6417,7 +5928,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>360</v>
+        <v>175</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>83</v>
@@ -6478,7 +5989,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>361</v>
+        <v>176</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>82</v>
@@ -6487,13 +5998,13 @@
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>18</v>
@@ -6565,7 +6076,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>362</v>
+        <v>177</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>83</v>
@@ -6574,13 +6085,13 @@
         <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H5" s="1"/>
       <c r="I5" s="1"/>
@@ -6873,13 +6384,13 @@
         <v>8</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="G4" s="1" t="s">
         <v>18</v>
@@ -6952,13 +6463,13 @@
         <v>8</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>126</v>
+        <v>107</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="G5" s="1"/>
       <c r="H5" s="1"/>
@@ -7008,8 +6519,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{19A79848-7E61-44B5-97E7-0F536B72AE4E}">
   <dimension ref="A1:AC3"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7105,7 +6616,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>103</v>
+        <v>233</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>16</v>
@@ -7183,6 +6694,12 @@
       </c>
     </row>
     <row ht="72" r="3" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>237</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
@@ -7190,16 +6707,16 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>72</v>
+        <v>235</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>19</v>
@@ -7268,7 +6785,7 @@
   <dimension ref="A1:AC3"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7364,7 +6881,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>104</v>
+        <v>205</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>66</v>
@@ -7441,6 +6958,12 @@
       </c>
     </row>
     <row ht="43.2" r="3" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
+        <v>206</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>66</v>
       </c>
@@ -7448,16 +6971,16 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>72</v>
+        <v>235</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>19</v>
@@ -7530,7 +7053,7 @@
   <dimension ref="A1:AF3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:AB3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7635,7 +7158,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>105</v>
+        <v>207</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>66</v>
@@ -7721,6 +7244,12 @@
       </c>
     </row>
     <row ht="72" r="3" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
+        <v>208</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>66</v>
       </c>
@@ -7728,16 +7257,16 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>72</v>
+        <v>235</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>19</v>
@@ -7805,7 +7334,7 @@
   <dimension ref="A1:AF3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:AB3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7910,7 +7439,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>209</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>66</v>
@@ -7996,6 +7525,12 @@
       </c>
     </row>
     <row ht="72" r="3" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
+        <v>210</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>66</v>
       </c>
@@ -8003,16 +7538,16 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>72</v>
+        <v>235</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>19</v>
@@ -8080,7 +7615,7 @@
   <dimension ref="A1:AF3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:AB3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8185,7 +7720,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>109</v>
+        <v>215</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>66</v>
@@ -8271,6 +7806,12 @@
       </c>
     </row>
     <row ht="72" r="3" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
+        <v>216</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>66</v>
       </c>
@@ -8278,16 +7819,16 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>19</v>
@@ -8355,7 +7896,7 @@
   <dimension ref="A1:AC3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:AB3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8451,7 +7992,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>211</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>16</v>
@@ -8529,6 +8070,12 @@
       </c>
     </row>
     <row ht="72" r="3" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
+        <v>212</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>66</v>
       </c>
@@ -8536,16 +8083,16 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>19</v>
@@ -8613,7 +8160,7 @@
   <dimension ref="A1:AC3"/>
   <sheetViews>
     <sheetView workbookViewId="0" zoomScaleNormal="100">
-      <selection activeCell="A3" sqref="A3:AB3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.44140625" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8709,7 +8256,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>108</v>
+        <v>213</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>66</v>
@@ -8786,6 +8333,12 @@
       </c>
     </row>
     <row ht="43.2" r="3" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
+        <v>214</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>66</v>
       </c>
@@ -8793,16 +8346,16 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>19</v>
@@ -8875,7 +8428,7 @@
   <dimension ref="A1:AF3"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:AB3"/>
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -8980,7 +8533,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>110</v>
+        <v>217</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>66</v>
@@ -9066,6 +8619,12 @@
       </c>
     </row>
     <row ht="72" r="3" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>81</v>
+      </c>
+      <c r="B3" t="s">
+        <v>218</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>66</v>
       </c>
@@ -9073,16 +8632,16 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H3" s="1" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="I3" s="1" t="s">
         <v>19</v>
@@ -9271,7 +8830,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>367</v>
+        <v>112</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>59</v>
@@ -9354,7 +8913,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>368</v>
+        <v>113</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>61</v>
@@ -9392,7 +8951,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>369</v>
+        <v>114</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>62</v>
@@ -9463,7 +9022,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>370</v>
+        <v>115</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>59</v>
@@ -9472,13 +9031,13 @@
         <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>18</v>
@@ -9546,7 +9105,7 @@
         <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>371</v>
+        <v>116</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>61</v>
@@ -9555,13 +9114,13 @@
         <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>26</v>
@@ -9584,7 +9143,7 @@
         <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>372</v>
+        <v>117</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>62</v>
@@ -9593,13 +9152,13 @@
         <v>8</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>18</v>
@@ -9757,7 +9316,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>311</v>
+        <v>136</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -9813,7 +9372,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>312</v>
+        <v>137</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -9869,7 +9428,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>313</v>
+        <v>138</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -9878,13 +9437,13 @@
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>79</v>
@@ -9925,7 +9484,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>314</v>
+        <v>139</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
@@ -9934,13 +9493,13 @@
         <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>78</v>
@@ -10091,7 +9650,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>315</v>
+        <v>140</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>66</v>
@@ -10157,7 +9716,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>316</v>
+        <v>141</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>68</v>
@@ -10223,7 +9782,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>317</v>
+        <v>142</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>66</v>
@@ -10232,13 +9791,13 @@
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>79</v>
@@ -10289,7 +9848,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>318</v>
+        <v>143</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>68</v>
@@ -10298,13 +9857,13 @@
         <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>78</v>
@@ -10465,7 +10024,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>319</v>
+        <v>144</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>66</v>
@@ -10531,7 +10090,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>320</v>
+        <v>145</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>68</v>
@@ -10597,7 +10156,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>321</v>
+        <v>146</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>66</v>
@@ -10606,13 +10165,13 @@
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>79</v>
@@ -10663,7 +10222,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>322</v>
+        <v>147</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>68</v>
@@ -10672,13 +10231,13 @@
         <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>78</v>
@@ -10830,7 +10389,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>307</v>
+        <v>132</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>68</v>
@@ -10887,7 +10446,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>308</v>
+        <v>133</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>68</v>
@@ -10944,7 +10503,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>309</v>
+        <v>134</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>68</v>
@@ -10953,13 +10512,13 @@
         <v>8</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H4" s="1" t="s">
         <v>79</v>
@@ -11001,7 +10560,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>310</v>
+        <v>135</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>68</v>
@@ -11010,13 +10569,13 @@
         <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>78</v>
@@ -11164,7 +10723,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>301</v>
+        <v>126</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>68</v>
@@ -11215,7 +10774,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>302</v>
+        <v>127</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>68</v>
@@ -11224,13 +10783,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -11376,7 +10935,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>303</v>
+        <v>128</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>68</v>
@@ -11436,7 +10995,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>304</v>
+        <v>129</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>68</v>
@@ -11445,13 +11004,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -11606,7 +11165,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>305</v>
+        <v>130</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>68</v>
@@ -11666,7 +11225,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>306</v>
+        <v>131</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>68</v>
@@ -11675,13 +11234,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -11827,7 +11386,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>299</v>
+        <v>124</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -11877,7 +11436,7 @@
         <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>300</v>
+        <v>125</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -11886,13 +11445,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>127</v>
+        <v>108</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -12028,7 +11587,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>112</v>
+        <v>221</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>16</v>
@@ -12084,6 +11643,12 @@
       </c>
     </row>
     <row ht="72" r="3" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>222</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
@@ -12091,13 +11656,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>79</v>
@@ -12252,7 +11817,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>114</v>
+        <v>225</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>66</v>
@@ -12314,6 +11879,12 @@
       </c>
     </row>
     <row ht="72" r="3" spans="1:31" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>226</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>66</v>
       </c>
@@ -12321,13 +11892,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>79</v>
@@ -12504,7 +12075,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>327</v>
+        <v>152</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>66</v>
@@ -12584,7 +12155,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>328</v>
+        <v>153</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>68</v>
@@ -12622,7 +12193,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>329</v>
+        <v>154</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>69</v>
@@ -12687,7 +12258,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>330</v>
+        <v>155</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>66</v>
@@ -12696,13 +12267,13 @@
         <v>8</v>
       </c>
       <c r="E5" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F5" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H5" s="1" t="s">
         <v>18</v>
@@ -12767,7 +12338,7 @@
         <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>331</v>
+        <v>156</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>68</v>
@@ -12776,13 +12347,13 @@
         <v>8</v>
       </c>
       <c r="E6" s="1" t="s">
-        <v>123</v>
+        <v>104</v>
       </c>
       <c r="F6" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="P6" s="1" t="s">
         <v>26</v>
@@ -12805,7 +12376,7 @@
         <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>332</v>
+        <v>157</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>69</v>
@@ -12814,13 +12385,13 @@
         <v>8</v>
       </c>
       <c r="E7" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F7" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H7" s="1" t="s">
         <v>18</v>
@@ -12972,7 +12543,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>113</v>
+        <v>223</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>66</v>
@@ -13025,6 +12596,12 @@
       </c>
     </row>
     <row ht="43.2" r="3" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>224</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>66</v>
       </c>
@@ -13032,13 +12609,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>128</v>
+        <v>109</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>79</v>
@@ -13195,7 +12772,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>115</v>
+        <v>227</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>66</v>
@@ -13261,7 +12838,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>115</v>
+        <v>228</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>66</v>
@@ -13273,10 +12850,10 @@
         <v>77</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>129</v>
+        <v>110</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>79</v>
@@ -13437,7 +13014,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>119</v>
+        <v>232</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>66</v>
@@ -13613,7 +13190,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>118</v>
+        <v>231</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>66</v>
@@ -13780,7 +13357,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>116</v>
+        <v>229</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>16</v>
@@ -13941,7 +13518,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>117</v>
+        <v>230</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>66</v>
@@ -14104,7 +13681,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>101</v>
+        <v>201</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>16</v>
@@ -14182,6 +13759,12 @@
       </c>
     </row>
     <row ht="72" r="3" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>202</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
@@ -14189,13 +13772,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>18</v>
@@ -14366,7 +13949,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>102</v>
+        <v>203</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>16</v>
@@ -14444,6 +14027,12 @@
       </c>
     </row>
     <row ht="72" r="3" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>204</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>16</v>
       </c>
@@ -14451,13 +14040,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>18</v>
@@ -14623,10 +14212,10 @@
     </row>
     <row ht="43.2" r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>111</v>
+        <v>219</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>68</v>
@@ -14675,6 +14264,12 @@
       <c r="AA2" s="1"/>
     </row>
     <row ht="43.2" r="3" spans="1:28" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>74</v>
+      </c>
+      <c r="B3" t="s">
+        <v>220</v>
+      </c>
       <c r="C3" s="1" t="s">
         <v>68</v>
       </c>
@@ -14682,13 +14277,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H3" s="1"/>
       <c r="I3" s="1"/>
@@ -14832,7 +14427,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>382</v>
+        <v>191</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>69</v>
@@ -14903,7 +14498,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>383</v>
+        <v>192</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>69</v>
@@ -14912,13 +14507,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>18</v>
@@ -15075,7 +14670,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>386</v>
+        <v>195</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>69</v>
@@ -15146,7 +14741,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>387</v>
+        <v>196</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>69</v>
@@ -15155,13 +14750,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>18</v>
@@ -15221,7 +14816,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A9E142F-4A51-4D5A-B6C1-BDE7AA487EEE}">
   <dimension ref="A1:AD3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
@@ -15406,13 +15001,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>18</v>
@@ -15585,7 +15180,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>390</v>
+        <v>199</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>59</v>
@@ -15669,7 +15264,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>391</v>
+        <v>200</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>59</v>
@@ -15678,13 +15273,13 @@
         <v>8</v>
       </c>
       <c r="E3" s="1" t="s">
-        <v>124</v>
+        <v>105</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>121</v>
+        <v>102</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>122</v>
+        <v>103</v>
       </c>
       <c r="H3" s="1" t="s">
         <v>18</v>

</xml_diff>

<commit_message>
Production Verification Script : User Management LInks and Reports Links
</commit_message>
<xml_diff>
--- a/KatalonData/IWPTestData/VRelay25Payments.xlsx
+++ b/KatalonData/IWPTestData/VRelay25Payments.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3680" uniqueCount="238">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3956" uniqueCount="307">
   <si>
     <t>Result</t>
   </si>
@@ -785,6 +785,213 @@
   </si>
   <si>
     <t>Mon Nov 04 22:07:50 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Nov 28 23:18:08 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Nov 28 23:36:16 IST 2024</t>
+  </si>
+  <si>
+    <t>Thu Nov 28 23:53:07 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 00:11:00 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 00:28:23 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 00:46:16 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 01:03:30 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 01:21:29 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 01:38:50 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 01:57:27 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 02:15:35 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 02:33:03 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 02:50:41 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 03:09:19 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 03:27:31 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 03:44:59 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 04:01:58 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 04:20:29 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 04:38:49 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 04:56:20 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 05:14:24 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 05:32:59 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 05:51:36 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 06:09:39 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 06:27:41 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 06:47:46 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 07:06:59 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 07:25:16 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 07:44:00 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 08:02:15 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 08:21:24 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 08:39:42 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 08:57:12 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 09:15:25 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 09:33:45 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 09:54:09 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 10:13:44 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 10:32:22 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 10:50:45 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 11:10:26 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 11:30:10 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 11:47:34 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 12:04:58 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 12:24:35 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 12:44:00 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 13:01:20 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 13:18:40 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 13:36:35 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 13:54:05 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 14:12:58 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 14:32:03 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 14:49:14 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 15:07:02 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 15:25:51 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 15:44:26 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 16:01:51 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 16:18:54 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 16:37:45 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 16:56:53 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 17:14:06 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 17:32:08 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 17:50:39 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 18:09:38 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 18:27:04 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 18:44:34 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 19:02:10 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 19:19:18 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 21:01:53 IST 2024</t>
+  </si>
+  <si>
+    <t>Fri Nov 29 21:35:12 IST 2024</t>
   </si>
 </sst>
 </file>
@@ -1321,7 +1528,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>182</v>
+        <v>300</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -1359,7 +1566,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>183</v>
+        <v>301</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>16</v>
@@ -1439,7 +1646,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>184</v>
+        <v>302</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>16</v>
@@ -1519,7 +1726,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>185</v>
+        <v>303</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>37</v>
@@ -1587,7 +1794,7 @@
         <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>186</v>
+        <v>304</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
@@ -3021,10 +3228,10 @@
     </row>
     <row ht="43.2" r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>158</v>
+        <v>272</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>66</v>
@@ -3102,10 +3309,10 @@
     </row>
     <row ht="43.2" r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>159</v>
+        <v>273</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>68</v>
@@ -3155,10 +3362,10 @@
     </row>
     <row ht="43.2" r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>160</v>
+        <v>274</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>66</v>
@@ -3236,10 +3443,10 @@
     </row>
     <row ht="43.2" r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
-        <v>161</v>
+        <v>275</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>68</v>
@@ -3395,10 +3602,10 @@
     </row>
     <row ht="72" r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>166</v>
+        <v>280</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -3449,10 +3656,10 @@
     </row>
     <row ht="72" r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>167</v>
+        <v>281</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>16</v>
@@ -3534,7 +3741,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>168</v>
+        <v>282</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -3588,7 +3795,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>169</v>
+        <v>283</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>16</v>
@@ -3777,7 +3984,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>170</v>
+        <v>288</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>82</v>
@@ -3864,7 +4071,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>171</v>
+        <v>289</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>83</v>
@@ -3922,10 +4129,10 @@
     </row>
     <row ht="72" r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>172</v>
+        <v>290</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>82</v>
@@ -4009,10 +4216,10 @@
     </row>
     <row ht="86.4" r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
-        <v>173</v>
+        <v>291</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>83</v>
@@ -4180,7 +4387,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>178</v>
+        <v>296</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>82</v>
@@ -4267,7 +4474,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>179</v>
+        <v>297</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>83</v>
@@ -4325,10 +4532,10 @@
     </row>
     <row ht="72" r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>180</v>
+        <v>298</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>82</v>
@@ -4412,10 +4619,10 @@
     </row>
     <row ht="86.4" r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
-        <v>181</v>
+        <v>299</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>83</v>
@@ -4574,10 +4781,10 @@
     </row>
     <row ht="72" r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>162</v>
+        <v>276</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -4628,10 +4835,10 @@
     </row>
     <row ht="72" r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>163</v>
+        <v>277</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>16</v>
@@ -4713,7 +4920,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>164</v>
+        <v>278</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -4767,7 +4974,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>165</v>
+        <v>279</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>16</v>
@@ -4947,10 +5154,10 @@
     </row>
     <row ht="43.2" r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>262</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>66</v>
@@ -5028,10 +5235,10 @@
     </row>
     <row ht="43.2" r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>149</v>
+        <v>263</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>68</v>
@@ -5081,10 +5288,10 @@
     </row>
     <row ht="43.2" r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>150</v>
+        <v>264</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>66</v>
@@ -5162,10 +5369,10 @@
     </row>
     <row ht="43.2" r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
-        <v>151</v>
+        <v>265</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>68</v>
@@ -5841,7 +6048,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>174</v>
+        <v>292</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>82</v>
@@ -5928,7 +6135,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>175</v>
+        <v>293</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>83</v>
@@ -5986,10 +6193,10 @@
     </row>
     <row ht="72" r="4" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>176</v>
+        <v>294</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>82</v>
@@ -6073,10 +6280,10 @@
     </row>
     <row ht="86.4" r="5" spans="1:30" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
-        <v>177</v>
+        <v>295</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>83</v>
@@ -9313,10 +9520,10 @@
     </row>
     <row ht="72" r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>136</v>
+        <v>250</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -9369,10 +9576,10 @@
     </row>
     <row ht="72" r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>137</v>
+        <v>251</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -9428,7 +9635,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>138</v>
+        <v>252</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -9484,7 +9691,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>139</v>
+        <v>253</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
@@ -9647,10 +9854,10 @@
     </row>
     <row ht="72" r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>140</v>
+        <v>254</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>66</v>
@@ -9713,10 +9920,10 @@
     </row>
     <row ht="72" r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>141</v>
+        <v>255</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>68</v>
@@ -9779,10 +9986,10 @@
     </row>
     <row ht="72" r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>142</v>
+        <v>256</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>66</v>
@@ -9845,10 +10052,10 @@
     </row>
     <row ht="72" r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
-        <v>143</v>
+        <v>257</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>68</v>
@@ -10021,10 +10228,10 @@
     </row>
     <row ht="72" r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>144</v>
+        <v>258</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>66</v>
@@ -10087,10 +10294,10 @@
     </row>
     <row ht="72" r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>145</v>
+        <v>259</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>68</v>
@@ -10153,10 +10360,10 @@
     </row>
     <row ht="72" r="4" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>146</v>
+        <v>260</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>66</v>
@@ -10219,10 +10426,10 @@
     </row>
     <row ht="72" r="5" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
-        <v>147</v>
+        <v>261</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>68</v>
@@ -10386,10 +10593,10 @@
     </row>
     <row ht="43.2" r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>132</v>
+        <v>246</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>68</v>
@@ -10443,10 +10650,10 @@
     </row>
     <row ht="43.2" r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>133</v>
+        <v>247</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>68</v>
@@ -10500,10 +10707,10 @@
     </row>
     <row ht="43.2" r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>134</v>
+        <v>248</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>68</v>
@@ -10557,10 +10764,10 @@
     </row>
     <row ht="43.2" r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
-        <v>135</v>
+        <v>249</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>68</v>
@@ -10720,10 +10927,10 @@
     </row>
     <row ht="72" r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>126</v>
+        <v>240</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>68</v>
@@ -10771,10 +10978,10 @@
     </row>
     <row ht="72" r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>127</v>
+        <v>241</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>68</v>
@@ -10932,10 +11139,10 @@
     </row>
     <row ht="72" r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>128</v>
+        <v>242</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>68</v>
@@ -10992,10 +11199,10 @@
     </row>
     <row ht="72" r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>129</v>
+        <v>243</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>68</v>
@@ -11162,10 +11369,10 @@
     </row>
     <row ht="72" r="2" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>130</v>
+        <v>244</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>68</v>
@@ -11222,10 +11429,10 @@
     </row>
     <row ht="72" r="3" spans="1:31" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>131</v>
+        <v>245</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>68</v>
@@ -11383,10 +11590,10 @@
     </row>
     <row ht="72" r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>306</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -11436,7 +11643,7 @@
         <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>125</v>
+        <v>239</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -12072,10 +12279,10 @@
     </row>
     <row ht="28.8" r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>152</v>
+        <v>266</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>66</v>
@@ -12152,10 +12359,10 @@
     </row>
     <row ht="28.8" r="3" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B3" t="s">
-        <v>153</v>
+        <v>267</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>68</v>
@@ -12190,10 +12397,10 @@
     </row>
     <row ht="43.2" r="4" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B4" t="s">
-        <v>154</v>
+        <v>268</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>69</v>
@@ -12255,10 +12462,10 @@
     </row>
     <row ht="28.8" r="5" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B5" t="s">
-        <v>155</v>
+        <v>269</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>66</v>
@@ -12335,10 +12542,10 @@
     </row>
     <row ht="28.8" r="6" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B6" t="s">
-        <v>156</v>
+        <v>270</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>68</v>
@@ -12373,10 +12580,10 @@
     </row>
     <row ht="43.2" r="7" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B7" t="s">
-        <v>157</v>
+        <v>271</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>69</v>

</xml_diff>

<commit_message>
Updated Vlink test cases
</commit_message>
<xml_diff>
--- a/KatalonData/IWPTestData/VRelay25Payments.xlsx
+++ b/KatalonData/IWPTestData/VRelay25Payments.xlsx
@@ -71,7 +71,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8439" uniqueCount="1430">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8735" uniqueCount="1504">
   <si>
     <t>Result</t>
   </si>
@@ -4361,6 +4361,228 @@
   </si>
   <si>
     <t>Fri Aug 08 04:17:11 IST 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 20:35:31 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 20:36:03 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 20:36:30 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 20:36:57 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 20:37:24 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 20:37:51 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 20:38:17 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 20:38:46 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:40:04 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:41:04 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:41:31 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:42:01 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:42:28 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:43:25 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:43:52 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:44:18 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:44:45 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:45:12 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:45:38 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:46:04 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:46:31 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:46:57 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:47:22 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:47:49 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:48:16 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:48:58 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:49:38 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:50:20 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:51:02 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:51:29 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:52:11 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:52:55 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:53:38 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:54:19 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:55:01 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:55:43 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:56:25 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:57:07 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:57:48 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:58:31 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:59:12 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 21:59:54 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:00:21 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:01:03 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:01:45 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:02:27 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:03:09 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:03:51 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:04:33 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:05:15 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:05:56 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:06:38 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:07:19 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:08:00 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:08:42 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:09:24 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:10:07 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:10:49 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:11:30 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:11:58 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:12:23 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:12:49 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:13:16 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:13:43 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:14:10 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:15:08 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:15:34 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:16:00 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:16:28 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:16:53 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:17:20 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:17:46 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:18:12 EDT 2025</t>
+  </si>
+  <si>
+    <t>Thu Aug 28 22:18:37 EDT 2025</t>
   </si>
 </sst>
 </file>
@@ -4894,10 +5116,10 @@
     </row>
     <row ht="28.8" r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>1349</v>
+        <v>1494</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -4935,7 +5157,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>1350</v>
+        <v>1495</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>16</v>
@@ -5015,7 +5237,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>1351</v>
+        <v>1496</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>16</v>
@@ -5095,7 +5317,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>1352</v>
+        <v>1497</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>37</v>
@@ -5163,7 +5385,7 @@
         <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>1353</v>
+        <v>1498</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>7</v>
@@ -5201,7 +5423,7 @@
         <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>1354</v>
+        <v>1499</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>16</v>
@@ -5281,7 +5503,7 @@
         <v>74</v>
       </c>
       <c r="B8" t="s">
-        <v>1355</v>
+        <v>1500</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>16</v>
@@ -5361,7 +5583,7 @@
         <v>74</v>
       </c>
       <c r="B9" t="s">
-        <v>1356</v>
+        <v>1501</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>37</v>
@@ -6612,7 +6834,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>1320</v>
+        <v>1459</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>66</v>
@@ -6693,7 +6915,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>1321</v>
+        <v>1460</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>68</v>
@@ -6746,7 +6968,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>1322</v>
+        <v>1461</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>66</v>
@@ -6827,7 +7049,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>1323</v>
+        <v>1462</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>68</v>
@@ -6986,7 +7208,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>1329</v>
+        <v>1467</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -7040,7 +7262,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>1330</v>
+        <v>1468</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>16</v>
@@ -7122,7 +7344,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>1331</v>
+        <v>1469</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -7176,7 +7398,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>1332</v>
+        <v>1470</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>16</v>
@@ -7365,7 +7587,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>1337</v>
+        <v>1476</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>82</v>
@@ -7452,7 +7674,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>1338</v>
+        <v>1477</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>83</v>
@@ -7513,7 +7735,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>1339</v>
+        <v>1478</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>82</v>
@@ -7600,7 +7822,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>1340</v>
+        <v>1479</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>83</v>
@@ -7768,7 +7990,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>1341</v>
+        <v>1484</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>82</v>
@@ -7855,7 +8077,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>1342</v>
+        <v>1485</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>83</v>
@@ -7916,7 +8138,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>1343</v>
+        <v>1486</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>82</v>
@@ -8003,7 +8225,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>1344</v>
+        <v>1487</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>83</v>
@@ -8165,7 +8387,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>1325</v>
+        <v>1463</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -8219,7 +8441,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>1326</v>
+        <v>1464</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>16</v>
@@ -8301,7 +8523,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>1327</v>
+        <v>1465</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -8355,7 +8577,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>1328</v>
+        <v>1466</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>16</v>
@@ -8538,7 +8760,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>1316</v>
+        <v>1454</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>66</v>
@@ -8619,7 +8841,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>1317</v>
+        <v>1455</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>68</v>
@@ -8672,7 +8894,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>1318</v>
+        <v>1456</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>66</v>
@@ -8753,7 +8975,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>1319</v>
+        <v>1457</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>68</v>
@@ -8937,7 +9159,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>1309</v>
+        <v>1471</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>59</v>
@@ -9429,7 +9651,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>1345</v>
+        <v>1480</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>82</v>
@@ -9516,7 +9738,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>1346</v>
+        <v>1481</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>83</v>
@@ -9577,7 +9799,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>1347</v>
+        <v>1482</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>82</v>
@@ -9664,7 +9886,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>1348</v>
+        <v>1483</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>83</v>
@@ -12422,7 +12644,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>1310</v>
+        <v>1488</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>59</v>
@@ -12505,7 +12727,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>1311</v>
+        <v>1489</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>61</v>
@@ -12543,7 +12765,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>1312</v>
+        <v>1490</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>62</v>
@@ -12614,7 +12836,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>1313</v>
+        <v>1491</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>59</v>
@@ -12697,7 +12919,7 @@
         <v>74</v>
       </c>
       <c r="B6" t="s">
-        <v>1314</v>
+        <v>1492</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>61</v>
@@ -12735,7 +12957,7 @@
         <v>74</v>
       </c>
       <c r="B7" t="s">
-        <v>1315</v>
+        <v>1493</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>62</v>
@@ -12905,10 +13127,10 @@
     </row>
     <row ht="72" r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>1361</v>
+        <v>1442</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>7</v>
@@ -12964,7 +13186,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>1362</v>
+        <v>1443</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
@@ -13020,7 +13242,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>1363</v>
+        <v>1444</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>7</v>
@@ -13076,7 +13298,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>1364</v>
+        <v>1445</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
@@ -13242,7 +13464,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>1365</v>
+        <v>1446</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>66</v>
@@ -13308,7 +13530,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>1366</v>
+        <v>1447</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>68</v>
@@ -13374,7 +13596,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>1367</v>
+        <v>1448</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>66</v>
@@ -13440,7 +13662,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>1368</v>
+        <v>1449</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>68</v>
@@ -13616,7 +13838,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>1369</v>
+        <v>1450</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>66</v>
@@ -13682,7 +13904,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>1370</v>
+        <v>1451</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>68</v>
@@ -13748,7 +13970,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>1371</v>
+        <v>1452</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>66</v>
@@ -13814,7 +14036,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>1372</v>
+        <v>1453</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>68</v>
@@ -13978,10 +14200,10 @@
     </row>
     <row ht="43.2" r="2" spans="1:28" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>74</v>
+        <v>81</v>
       </c>
       <c r="B2" t="s">
-        <v>1357</v>
+        <v>1438</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>68</v>
@@ -14038,7 +14260,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>1358</v>
+        <v>1439</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>68</v>
@@ -14095,7 +14317,7 @@
         <v>74</v>
       </c>
       <c r="B4" t="s">
-        <v>1359</v>
+        <v>1440</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>68</v>
@@ -14152,7 +14374,7 @@
         <v>74</v>
       </c>
       <c r="B5" t="s">
-        <v>1360</v>
+        <v>1441</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>68</v>
@@ -15671,7 +15893,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>1324</v>
+        <v>1458</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>66</v>
@@ -17545,7 +17767,7 @@
         <v>74</v>
       </c>
       <c r="B2" t="s">
-        <v>1391</v>
+        <v>1502</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>16</v>
@@ -17627,7 +17849,7 @@
         <v>74</v>
       </c>
       <c r="B3" t="s">
-        <v>1392</v>
+        <v>1503</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>16</v>

</xml_diff>